<commit_message>
Collector V2.0 - Parse기능 포함
</commit_message>
<xml_diff>
--- a/Collector_device_src.xlsx
+++ b/Collector_device_src.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\12. Python Src\LogCollector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E607A082-2D9C-4561-9C74-59E65C5D9CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1FC8E0-926E-4DEA-B15E-A457DDE2F6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Hostname:String:Required</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,23 +65,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FIB4</t>
-  </si>
-  <si>
-    <t>192.168.10.185</t>
+    <t>NXOS1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.105</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>!@Etech123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CISCO_NXOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.62</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ServerFarm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fusion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A_EDGE1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdadmin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Qwer12345!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CISCO_XE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +134,14 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -111,17 +162,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A2:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -445,7 +501,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -459,19 +515,101 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{131547E1-87FC-4CB2-AF6C-28B4DF98136B}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{F7B49873-2B18-4510-8E4F-0D59BAF4D6A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>